<commit_message>
Added more data to the snowballing data frame - 1600 obs / 102 studies
</commit_message>
<xml_diff>
--- a/Data/Snowballing/snowballing_Literature.xlsx
+++ b/Data/Snowballing/snowballing_Literature.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10121" uniqueCount="5365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10217" uniqueCount="5375">
   <si>
     <t>Number</t>
   </si>
@@ -16787,14 +16787,44 @@
     <t>Journal of Econometrics</t>
   </si>
   <si>
-    <t>MASTER</t>
+    <t>much theory</t>
+  </si>
+  <si>
+    <t>DISCONTINUITY</t>
+  </si>
+  <si>
+    <t>PART OF MAIN QUERY</t>
+  </si>
+  <si>
+    <t>IQ ONLY</t>
+  </si>
+  <si>
+    <t>Focuses purely on ability, no returns to schooling (except for meta data)</t>
+  </si>
+  <si>
+    <t>Effect of a reform on years of schooling / immigration</t>
+  </si>
+  <si>
+    <t>Math reform instead of years of schooling</t>
+  </si>
+  <si>
+    <t>wrong flag, collected later as a part of snowballing literature, also brilliant for literature, primary study also</t>
+  </si>
+  <si>
+    <t>cool theory on abiliity bias, so really 1, but no data for 1, only 3</t>
+  </si>
+  <si>
+    <t>TWINS</t>
+  </si>
+  <si>
+    <t>from snowballing query</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -16859,6 +16889,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -17117,7 +17155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -17168,12 +17206,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="60">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8CDC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6161"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8CDC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -17413,27 +17558,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA8CDC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17854,8 +17978,8 @@
   <dimension ref="A1:Y575"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17931,14 +18055,14 @@
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!S1</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5039</v>
       </c>
       <c r="U1" s="29">
         <f>COUNTIF($L$2:$L$575, "&lt;&gt; ") +Twins!V1</f>
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -18267,6 +18391,12 @@
       <c r="O7" s="7" t="s">
         <v>5029</v>
       </c>
+      <c r="P7" t="s">
+        <v>5371</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>904</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -44499,59 +44629,59 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="48" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="47" priority="20">
+    <cfRule type="containsBlanks" dxfId="58" priority="20">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N601">
-    <cfRule type="containsText" dxfId="46" priority="11" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="57" priority="11" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",L2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="45" priority="12" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="56" priority="12" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",L2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="55" priority="13" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O601 P136 P146 P151 P161 P163 P177 P187 P189:P190">
-    <cfRule type="containsBlanks" dxfId="43" priority="22">
+    <cfRule type="containsBlanks" dxfId="54" priority="22">
       <formula>LEN(TRIM(O2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O601 P177 P187 P189:P190">
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="53" priority="8" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="52" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q10 Q16:Q1048576 R11:R15">
-    <cfRule type="duplicateValues" dxfId="40" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="39" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="38" priority="23">
+    <cfRule type="containsBlanks" dxfId="49" priority="23">
       <formula>LEN(TRIM(R6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8">
-    <cfRule type="cellIs" dxfId="37" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="47" priority="18" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="duplicateValues" dxfId="35" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="5"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K160" r:id="rId1" location="page=11"/>
@@ -44569,8 +44699,8 @@
   <dimension ref="A1:AC575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25:S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44647,20 +44777,22 @@
       <c r="S1" s="25" t="s">
         <v>5137</v>
       </c>
-      <c r="T1" s="31"/>
+      <c r="T1" s="44" t="s">
+        <v>5145</v>
+      </c>
       <c r="U1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="V1" s="29">
         <f>COUNTIFS($Q:$Q, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X1" s="28" t="s">
         <v>5039</v>
       </c>
       <c r="Y1" s="29">
         <f>COUNTIF($P:$P, "YES")</f>
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="Z1" s="31"/>
       <c r="AA1" s="31"/>
@@ -44780,7 +44912,7 @@
         <v>5029</v>
       </c>
       <c r="P3" t="s">
-        <v>5364</v>
+        <v>5366</v>
       </c>
       <c r="Q3" s="42" t="s">
         <v>963</v>
@@ -44838,10 +44970,18 @@
       <c r="O4" t="s">
         <v>5029</v>
       </c>
+      <c r="P4" t="s">
+        <v>963</v>
+      </c>
       <c r="Q4" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S4" s="7"/>
+      <c r="R4" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S4" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -44889,10 +45029,18 @@
       <c r="O5" t="s">
         <v>5029</v>
       </c>
+      <c r="P5" t="s">
+        <v>963</v>
+      </c>
       <c r="Q5" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S5" s="7"/>
+      <c r="R5" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S5" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -44940,16 +45088,27 @@
       <c r="O6" t="s">
         <v>5029</v>
       </c>
-      <c r="Q6" s="42" t="s">
-        <v>963</v>
-      </c>
-      <c r="S6" s="7"/>
+      <c r="P6" s="43" t="s">
+        <v>967</v>
+      </c>
+      <c r="Q6" s="43" t="s">
+        <v>967</v>
+      </c>
+      <c r="R6" s="43" t="s">
+        <v>966</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>5029</v>
+      </c>
+      <c r="T6" t="s">
+        <v>5364</v>
+      </c>
       <c r="U6" s="2" t="s">
         <v>5143</v>
       </c>
       <c r="V6">
         <f>COUNTIF($P:$P, "YES")</f>
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
@@ -44998,16 +45157,24 @@
       <c r="O7" t="s">
         <v>5029</v>
       </c>
+      <c r="P7" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q7" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S7" s="7"/>
+      <c r="R7" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S7" s="7">
+        <v>1</v>
+      </c>
       <c r="U7" s="2" t="s">
         <v>5140</v>
       </c>
       <c r="V7">
         <f>COUNTIFS($R:$R, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
@@ -45056,10 +45223,18 @@
       <c r="O8" t="s">
         <v>5029</v>
       </c>
+      <c r="P8" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q8" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S8" s="7"/>
+      <c r="R8" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S8" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -45107,10 +45282,18 @@
       <c r="O9" t="s">
         <v>5029</v>
       </c>
+      <c r="P9" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q9" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S9" s="7"/>
+      <c r="R9" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S9" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -45158,10 +45341,18 @@
       <c r="O10" t="s">
         <v>5029</v>
       </c>
+      <c r="P10" s="43" t="s">
+        <v>5365</v>
+      </c>
       <c r="Q10" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S10" s="7"/>
+      <c r="R10" s="43" t="s">
+        <v>966</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="11" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
@@ -45209,10 +45400,18 @@
       <c r="O11" s="40" t="s">
         <v>5029</v>
       </c>
+      <c r="P11" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q11" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S11" s="41"/>
+      <c r="R11" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S11" s="41">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -45260,10 +45459,18 @@
       <c r="O12" t="s">
         <v>5029</v>
       </c>
+      <c r="P12" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q12" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S12" s="7"/>
+      <c r="R12" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S12" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -45311,10 +45518,21 @@
       <c r="O13" t="s">
         <v>5029</v>
       </c>
+      <c r="P13" s="43" t="s">
+        <v>5367</v>
+      </c>
       <c r="Q13" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S13" s="7"/>
+      <c r="R13" s="43" t="s">
+        <v>966</v>
+      </c>
+      <c r="S13" s="7">
+        <v>1</v>
+      </c>
+      <c r="T13" t="s">
+        <v>5368</v>
+      </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -45362,10 +45580,18 @@
       <c r="O14" t="s">
         <v>5029</v>
       </c>
+      <c r="P14" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q14" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S14" s="7"/>
+      <c r="R14" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S14" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -45413,10 +45639,21 @@
       <c r="O15" t="s">
         <v>5029</v>
       </c>
+      <c r="P15" s="43" t="s">
+        <v>966</v>
+      </c>
       <c r="Q15" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S15" s="7"/>
+      <c r="R15" s="43" t="s">
+        <v>966</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>5029</v>
+      </c>
+      <c r="T15" t="s">
+        <v>5369</v>
+      </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -45464,12 +45701,20 @@
       <c r="O16" t="s">
         <v>5029</v>
       </c>
+      <c r="P16" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q16" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S16" s="7"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R16" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S16" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -45515,12 +45760,20 @@
       <c r="O17" t="s">
         <v>5029</v>
       </c>
+      <c r="P17" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q17" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S17" s="7"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R17" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S17" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -45566,12 +45819,20 @@
       <c r="O18" t="s">
         <v>5029</v>
       </c>
+      <c r="P18" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q18" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S18" s="7"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R18" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S18" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -45617,12 +45878,20 @@
       <c r="O19" t="s">
         <v>5029</v>
       </c>
+      <c r="P19" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q19" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S19" s="7"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R19" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S19" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -45668,12 +45937,20 @@
       <c r="O20" t="s">
         <v>5029</v>
       </c>
+      <c r="P20" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q20" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S20" s="7"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R20" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S20" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -45719,12 +45996,20 @@
       <c r="O21" t="s">
         <v>5029</v>
       </c>
+      <c r="P21" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q21" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S21" s="7"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R21" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S21" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -45747,7 +46032,7 @@
         <v>5029</v>
       </c>
       <c r="H22" t="s">
-        <v>167</v>
+        <v>253</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -45770,12 +46055,20 @@
       <c r="O22" t="s">
         <v>5029</v>
       </c>
+      <c r="P22" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q22" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S22" s="7"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R22" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S22" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -45821,12 +46114,23 @@
       <c r="O23" t="s">
         <v>5029</v>
       </c>
+      <c r="P23" s="43" t="s">
+        <v>966</v>
+      </c>
       <c r="Q23" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S23" s="7"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R23" s="43" t="s">
+        <v>966</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>5029</v>
+      </c>
+      <c r="T23" t="s">
+        <v>5370</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -45872,12 +46176,20 @@
       <c r="O24" t="s">
         <v>5029</v>
       </c>
+      <c r="P24" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q24" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S24" s="7"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R24" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S24" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -45923,12 +46235,20 @@
       <c r="O25" t="s">
         <v>5029</v>
       </c>
+      <c r="P25" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q25" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S25" s="7"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R25" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -45974,12 +46294,20 @@
       <c r="O26" t="s">
         <v>5029</v>
       </c>
+      <c r="P26" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q26" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S26" s="7"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R26" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S26" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -46025,12 +46353,20 @@
       <c r="O27" t="s">
         <v>5029</v>
       </c>
+      <c r="P27" s="43" t="s">
+        <v>963</v>
+      </c>
       <c r="Q27" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S27" s="7"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R27" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S27" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -46076,12 +46412,20 @@
       <c r="O28" t="s">
         <v>5029</v>
       </c>
+      <c r="P28" t="s">
+        <v>963</v>
+      </c>
       <c r="Q28" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S28" s="7"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R28" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S28" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -46127,12 +46471,20 @@
       <c r="O29" t="s">
         <v>5029</v>
       </c>
+      <c r="P29" t="s">
+        <v>966</v>
+      </c>
       <c r="Q29" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S29" s="7"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R29" s="43" t="s">
+        <v>966</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>5029</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -46178,12 +46530,23 @@
       <c r="O30" t="s">
         <v>5029</v>
       </c>
+      <c r="P30" t="s">
+        <v>963</v>
+      </c>
       <c r="Q30" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S30" s="7"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R30" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S30" s="7">
+        <v>3</v>
+      </c>
+      <c r="T30" t="s">
+        <v>5372</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -46229,12 +46592,20 @@
       <c r="O31" t="s">
         <v>5029</v>
       </c>
+      <c r="P31" t="s">
+        <v>963</v>
+      </c>
       <c r="Q31" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S31" s="7"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R31" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S31" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -46280,10 +46651,18 @@
       <c r="O32" t="s">
         <v>5029</v>
       </c>
+      <c r="P32" t="s">
+        <v>963</v>
+      </c>
       <c r="Q32" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S32" s="7"/>
+      <c r="R32" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S32" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
@@ -46331,10 +46710,18 @@
       <c r="O33" t="s">
         <v>5029</v>
       </c>
+      <c r="P33" t="s">
+        <v>963</v>
+      </c>
       <c r="Q33" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S33" s="7"/>
+      <c r="R33" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S33" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -46382,10 +46769,18 @@
       <c r="O34" t="s">
         <v>5029</v>
       </c>
+      <c r="P34" t="s">
+        <v>5373</v>
+      </c>
       <c r="Q34" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S34" s="7"/>
+      <c r="R34" s="43" t="s">
+        <v>966</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -46433,10 +46828,18 @@
       <c r="O35" t="s">
         <v>5029</v>
       </c>
+      <c r="P35" t="s">
+        <v>963</v>
+      </c>
       <c r="Q35" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S35" s="7"/>
+      <c r="R35" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S35" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="36" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40">
@@ -46484,10 +46887,18 @@
       <c r="O36" s="40" t="s">
         <v>5029</v>
       </c>
+      <c r="P36" t="s">
+        <v>963</v>
+      </c>
       <c r="Q36" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S36" s="41"/>
+      <c r="R36" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S36" s="41">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40">
@@ -46535,10 +46946,18 @@
       <c r="O37" s="40" t="s">
         <v>5029</v>
       </c>
+      <c r="P37" t="s">
+        <v>963</v>
+      </c>
       <c r="Q37" s="42" t="s">
         <v>963</v>
       </c>
-      <c r="S37" s="41"/>
+      <c r="R37" s="43" t="s">
+        <v>963</v>
+      </c>
+      <c r="S37" s="41">
+        <v>4</v>
+      </c>
     </row>
     <row r="38" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
@@ -49069,43 +49488,43 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="34" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="33" priority="13">
+    <cfRule type="containsBlanks" dxfId="44" priority="13">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:R601">
-    <cfRule type="containsText" dxfId="32" priority="8" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",P2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="31" priority="9" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="12" priority="9" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",P2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",P2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S601">
-    <cfRule type="containsBlanks" dxfId="29" priority="15">
+    <cfRule type="containsBlanks" dxfId="43" priority="15">
       <formula>LEN(TRIM(S2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S601">
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="6" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="41" priority="7" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",S2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U2">
-    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1">
-    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -49116,10 +49535,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49184,14 +49603,14 @@
       </c>
       <c r="S1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5039</v>
       </c>
       <c r="V1" s="29">
         <f>COUNTIF($M$2:$M$573, "YES")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="W1" s="31"/>
       <c r="X1" s="31"/>
@@ -49467,7 +49886,7 @@
       </c>
       <c r="S6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="X6" t="s">
         <v>5076</v>
@@ -50076,89 +50495,187 @@
       <c r="O18" t="s">
         <v>966</v>
       </c>
-      <c r="P18" s="7">
+      <c r="P18">
         <v>1</v>
       </c>
       <c r="Q18" t="s">
         <v>5146</v>
       </c>
     </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>399</v>
+      </c>
+      <c r="C19" t="s">
+        <v>400</v>
+      </c>
+      <c r="D19">
+        <v>1999</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5278</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5279</v>
+      </c>
+      <c r="G19" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H19">
+        <v>177</v>
+      </c>
+      <c r="I19" t="s">
+        <v>5029</v>
+      </c>
+      <c r="J19" t="s">
+        <v>5029</v>
+      </c>
+      <c r="K19" t="s">
+        <v>5029</v>
+      </c>
+      <c r="L19" t="s">
+        <v>399</v>
+      </c>
+      <c r="M19" t="s">
+        <v>963</v>
+      </c>
+      <c r="N19" t="s">
+        <v>963</v>
+      </c>
+      <c r="O19" t="s">
+        <v>966</v>
+      </c>
+      <c r="P19" t="s">
+        <v>5029</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>5374</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="24" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="23" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="containsBlanks" dxfId="22" priority="22">
+    <cfRule type="containsBlanks" dxfId="36" priority="33">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="containsBlanks" dxfId="21" priority="11">
+    <cfRule type="containsBlanks" dxfId="35" priority="22">
       <formula>LEN(TRIM(F18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H17 H19:H1048576">
-    <cfRule type="containsBlanks" dxfId="20" priority="23">
+  <conditionalFormatting sqref="H1:H17 H20:H1048576">
+    <cfRule type="containsBlanks" dxfId="34" priority="34">
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="duplicateValues" dxfId="19" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O18">
-    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="31" priority="19" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="16" priority="9" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="30" priority="20" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="29" priority="21" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O18">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="17" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="27" priority="18" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",O18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O18:P18">
-    <cfRule type="containsBlanks" dxfId="12" priority="4">
+    <cfRule type="containsBlanks" dxfId="26" priority="15">
       <formula>LEN(TRIM(O18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="between">
+  <conditionalFormatting sqref="P1:P18 P20:P1048576">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="24" priority="14" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1 Q4">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="28" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="18" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",Q1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R2">
-    <cfRule type="duplicateValues" dxfId="7" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="duplicateValues" dxfId="6" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="containsBlanks" dxfId="9" priority="11">
+      <formula>LEN(TRIM(F19))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19">
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M19:O19">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="PRIMARY STUDY">
+      <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M19)))</formula>
+    </cfRule>
+    <cfRule type="notContainsText" dxfId="6" priority="9" operator="notContains" text="YES">
+      <formula>ISERROR(SEARCH("YES",M19))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",M19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O19">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
+      <formula>1</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",O19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O19:P19">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
+      <formula>LEN(TRIM(O19))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P19">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>1</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",P19)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -59051,10 +59568,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1 A1:K251">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>$K1=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="18" priority="9">
       <formula>$J1=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -66999,10 +67516,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:J253 J257 J259:J1048576">
-    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="17" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67019,10 +67536,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",M17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",M17)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added more data to the snowballing literature
</commit_message>
<xml_diff>
--- a/Data/Snowballing/snowballing_Literature.xlsx
+++ b/Data/Snowballing/snowballing_Literature.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcala\temp\master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Data\Snowballing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E133AF0F-E218-44C4-8672-6FA0EFC4637C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -23,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Query literature'!$A$1:$Y$575</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Snowballing!$A$1:$AC$575</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,12 +42,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Petr Čala</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -125,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -151,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -177,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -203,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -229,7 +230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T4" authorId="0" shapeId="0">
+    <comment ref="T4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -255,7 +256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P11" authorId="0" shapeId="0">
+    <comment ref="P11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -286,12 +287,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Petr Čala</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -317,7 +318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -343,7 +344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -370,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -396,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -422,7 +423,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -448,7 +449,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U6" authorId="0" shapeId="0">
+    <comment ref="U6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -479,12 +480,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Petr Čala</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -510,7 +511,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -536,7 +537,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -563,7 +564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -589,7 +590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -615,7 +616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R6" authorId="0" shapeId="0">
+    <comment ref="R6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -646,12 +647,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Petr Čala</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -671,14 +672,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -693,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10217" uniqueCount="5375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10224" uniqueCount="5376">
   <si>
     <t>Number</t>
   </si>
@@ -16818,12 +16819,15 @@
   </si>
   <si>
     <t>from snowballing query</t>
+  </si>
+  <si>
+    <t>REPLICATION OF CARD(1995)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -17155,7 +17159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -17202,123 +17206,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA8CDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6161"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA8CDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="51">
     <dxf>
       <fill>
         <patternFill>
@@ -17476,6 +17371,17 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFAACAC"/>
@@ -17541,6 +17447,24 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFAACAC"/>
@@ -17557,7 +17481,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8CDC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17973,13 +17911,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y575"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P38" sqref="P38"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44629,64 +44567,64 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="59" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="58" priority="20">
+    <cfRule type="containsBlanks" dxfId="49" priority="20">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N601">
-    <cfRule type="containsText" dxfId="57" priority="11" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="48" priority="11" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",L2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="56" priority="12" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="47" priority="12" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",L2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="13" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="46" priority="13" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O601 P136 P146 P151 P161 P163 P177 P187 P189:P190">
-    <cfRule type="containsBlanks" dxfId="54" priority="22">
+    <cfRule type="containsBlanks" dxfId="45" priority="22">
       <formula>LEN(TRIM(O2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O601 P177 P187 P189:P190">
-    <cfRule type="cellIs" dxfId="53" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="44" priority="8" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="43" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q10 Q16:Q1048576 R11:R15">
-    <cfRule type="duplicateValues" dxfId="51" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="50" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="49" priority="23">
+    <cfRule type="containsBlanks" dxfId="40" priority="23">
       <formula>LEN(TRIM(R6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8">
-    <cfRule type="cellIs" dxfId="48" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="38" priority="18" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="duplicateValues" dxfId="46" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="5"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="K160" r:id="rId1" location="page=11"/>
-    <hyperlink ref="K9" r:id="rId2"/>
-    <hyperlink ref="J13" r:id="rId3" display="https://books.google.com/books?hl=en&amp;lr=&amp;id=xHdLezAGFFMC&amp;oi=fnd&amp;pg=PP13&amp;dq=(%22ability+bias%22+OR+%22intelligence+bias%22)+AND+(%22private+returns%22)+AND+(%22income%22+OR+%22earnings%22)+AND+(%22schooling%22+OR+%22education%22)&amp;ots=AMWBbfJpWa&amp;sig=HzNyY_GdLkNjo-PvjNkJ8XDbCMo"/>
+    <hyperlink ref="K160" r:id="rId1" location="page=11" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J13" r:id="rId3" display="https://books.google.com/books?hl=en&amp;lr=&amp;id=xHdLezAGFFMC&amp;oi=fnd&amp;pg=PP13&amp;dq=(%22ability+bias%22+OR+%22intelligence+bias%22)+AND+(%22private+returns%22)+AND+(%22income%22+OR+%22earnings%22)+AND+(%22schooling%22+OR+%22education%22)&amp;ots=AMWBbfJpWa&amp;sig=HzNyY_GdLkNjo-PvjNkJ8XDbCMo" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId4"/>
@@ -44695,12 +44633,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25:S25"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44777,7 +44715,7 @@
       <c r="S1" s="25" t="s">
         <v>5137</v>
       </c>
-      <c r="T1" s="44" t="s">
+      <c r="T1" s="40" t="s">
         <v>5145</v>
       </c>
       <c r="U1" s="28" t="s">
@@ -44792,7 +44730,7 @@
       </c>
       <c r="Y1" s="29">
         <f>COUNTIF($P:$P, "YES")</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Z1" s="31"/>
       <c r="AA1" s="31"/>
@@ -44914,10 +44852,10 @@
       <c r="P3" t="s">
         <v>5366</v>
       </c>
-      <c r="Q3" s="42" t="s">
+      <c r="Q3" t="s">
         <v>963</v>
       </c>
-      <c r="R3" s="43" t="s">
+      <c r="R3" t="s">
         <v>966</v>
       </c>
       <c r="S3" s="7" t="s">
@@ -44973,10 +44911,10 @@
       <c r="P4" t="s">
         <v>963</v>
       </c>
-      <c r="Q4" s="42" t="s">
+      <c r="Q4" t="s">
         <v>963</v>
       </c>
-      <c r="R4" s="43" t="s">
+      <c r="R4" t="s">
         <v>963</v>
       </c>
       <c r="S4" s="7">
@@ -45032,10 +44970,10 @@
       <c r="P5" t="s">
         <v>963</v>
       </c>
-      <c r="Q5" s="42" t="s">
+      <c r="Q5" t="s">
         <v>963</v>
       </c>
-      <c r="R5" s="43" t="s">
+      <c r="R5" t="s">
         <v>963</v>
       </c>
       <c r="S5" s="7">
@@ -45088,13 +45026,13 @@
       <c r="O6" t="s">
         <v>5029</v>
       </c>
-      <c r="P6" s="43" t="s">
+      <c r="P6" t="s">
         <v>967</v>
       </c>
-      <c r="Q6" s="43" t="s">
+      <c r="Q6" t="s">
         <v>967</v>
       </c>
-      <c r="R6" s="43" t="s">
+      <c r="R6" t="s">
         <v>966</v>
       </c>
       <c r="S6" s="7" t="s">
@@ -45108,7 +45046,7 @@
       </c>
       <c r="V6">
         <f>COUNTIF($P:$P, "YES")</f>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
@@ -45157,13 +45095,13 @@
       <c r="O7" t="s">
         <v>5029</v>
       </c>
-      <c r="P7" s="43" t="s">
+      <c r="P7" t="s">
         <v>963</v>
       </c>
-      <c r="Q7" s="42" t="s">
+      <c r="Q7" t="s">
         <v>963</v>
       </c>
-      <c r="R7" s="43" t="s">
+      <c r="R7" t="s">
         <v>963</v>
       </c>
       <c r="S7" s="7">
@@ -45174,7 +45112,7 @@
       </c>
       <c r="V7">
         <f>COUNTIFS($R:$R, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
@@ -45223,13 +45161,13 @@
       <c r="O8" t="s">
         <v>5029</v>
       </c>
-      <c r="P8" s="43" t="s">
+      <c r="P8" t="s">
         <v>963</v>
       </c>
-      <c r="Q8" s="42" t="s">
+      <c r="Q8" t="s">
         <v>963</v>
       </c>
-      <c r="R8" s="43" t="s">
+      <c r="R8" t="s">
         <v>963</v>
       </c>
       <c r="S8" s="7">
@@ -45282,13 +45220,13 @@
       <c r="O9" t="s">
         <v>5029</v>
       </c>
-      <c r="P9" s="43" t="s">
+      <c r="P9" t="s">
         <v>963</v>
       </c>
-      <c r="Q9" s="42" t="s">
+      <c r="Q9" t="s">
         <v>963</v>
       </c>
-      <c r="R9" s="43" t="s">
+      <c r="R9" t="s">
         <v>963</v>
       </c>
       <c r="S9" s="7">
@@ -45341,75 +45279,75 @@
       <c r="O10" t="s">
         <v>5029</v>
       </c>
-      <c r="P10" s="43" t="s">
+      <c r="P10" t="s">
         <v>5365</v>
       </c>
-      <c r="Q10" s="42" t="s">
+      <c r="Q10" t="s">
         <v>963</v>
       </c>
-      <c r="R10" s="43" t="s">
+      <c r="R10" t="s">
         <v>966</v>
       </c>
       <c r="S10" s="7" t="s">
         <v>5029</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" t="s">
         <v>5199</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" t="s">
         <v>5200</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11">
         <v>2014</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" t="s">
         <v>5201</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" t="s">
         <v>5202</v>
       </c>
-      <c r="G11" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H11" s="40" t="s">
+      <c r="G11" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H11" t="s">
         <v>253</v>
       </c>
-      <c r="I11" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" s="40" t="s">
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
         <v>5349</v>
       </c>
-      <c r="K11" s="40" t="s">
+      <c r="K11" t="s">
         <v>5349</v>
       </c>
-      <c r="L11" s="40">
+      <c r="L11">
         <v>17</v>
       </c>
-      <c r="M11" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N11" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O11" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="P11" s="43" t="s">
+      <c r="M11" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N11" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O11" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P11" t="s">
         <v>963</v>
       </c>
-      <c r="Q11" s="42" t="s">
+      <c r="Q11" t="s">
         <v>963</v>
       </c>
-      <c r="R11" s="43" t="s">
+      <c r="R11" t="s">
         <v>963</v>
       </c>
-      <c r="S11" s="41">
+      <c r="S11" s="7">
         <v>1</v>
       </c>
     </row>
@@ -45459,13 +45397,13 @@
       <c r="O12" t="s">
         <v>5029</v>
       </c>
-      <c r="P12" s="43" t="s">
+      <c r="P12" t="s">
         <v>963</v>
       </c>
-      <c r="Q12" s="42" t="s">
+      <c r="Q12" t="s">
         <v>963</v>
       </c>
-      <c r="R12" s="43" t="s">
+      <c r="R12" t="s">
         <v>963</v>
       </c>
       <c r="S12" s="7">
@@ -45518,13 +45456,13 @@
       <c r="O13" t="s">
         <v>5029</v>
       </c>
-      <c r="P13" s="43" t="s">
+      <c r="P13" t="s">
         <v>5367</v>
       </c>
-      <c r="Q13" s="42" t="s">
+      <c r="Q13" t="s">
         <v>963</v>
       </c>
-      <c r="R13" s="43" t="s">
+      <c r="R13" t="s">
         <v>966</v>
       </c>
       <c r="S13" s="7">
@@ -45580,13 +45518,13 @@
       <c r="O14" t="s">
         <v>5029</v>
       </c>
-      <c r="P14" s="43" t="s">
+      <c r="P14" t="s">
         <v>963</v>
       </c>
-      <c r="Q14" s="42" t="s">
+      <c r="Q14" t="s">
         <v>963</v>
       </c>
-      <c r="R14" s="43" t="s">
+      <c r="R14" t="s">
         <v>963</v>
       </c>
       <c r="S14" s="7">
@@ -45639,13 +45577,13 @@
       <c r="O15" t="s">
         <v>5029</v>
       </c>
-      <c r="P15" s="43" t="s">
+      <c r="P15" t="s">
         <v>966</v>
       </c>
-      <c r="Q15" s="42" t="s">
+      <c r="Q15" t="s">
         <v>963</v>
       </c>
-      <c r="R15" s="43" t="s">
+      <c r="R15" t="s">
         <v>966</v>
       </c>
       <c r="S15" s="7" t="s">
@@ -45701,13 +45639,13 @@
       <c r="O16" t="s">
         <v>5029</v>
       </c>
-      <c r="P16" s="43" t="s">
+      <c r="P16" t="s">
         <v>963</v>
       </c>
-      <c r="Q16" s="42" t="s">
+      <c r="Q16" t="s">
         <v>963</v>
       </c>
-      <c r="R16" s="43" t="s">
+      <c r="R16" t="s">
         <v>963</v>
       </c>
       <c r="S16" s="7">
@@ -45760,13 +45698,13 @@
       <c r="O17" t="s">
         <v>5029</v>
       </c>
-      <c r="P17" s="43" t="s">
+      <c r="P17" t="s">
         <v>963</v>
       </c>
-      <c r="Q17" s="42" t="s">
+      <c r="Q17" t="s">
         <v>963</v>
       </c>
-      <c r="R17" s="43" t="s">
+      <c r="R17" t="s">
         <v>963</v>
       </c>
       <c r="S17" s="7">
@@ -45819,13 +45757,13 @@
       <c r="O18" t="s">
         <v>5029</v>
       </c>
-      <c r="P18" s="43" t="s">
+      <c r="P18" t="s">
         <v>963</v>
       </c>
-      <c r="Q18" s="42" t="s">
+      <c r="Q18" t="s">
         <v>963</v>
       </c>
-      <c r="R18" s="43" t="s">
+      <c r="R18" t="s">
         <v>963</v>
       </c>
       <c r="S18" s="7">
@@ -45878,13 +45816,13 @@
       <c r="O19" t="s">
         <v>5029</v>
       </c>
-      <c r="P19" s="43" t="s">
+      <c r="P19" t="s">
         <v>963</v>
       </c>
-      <c r="Q19" s="42" t="s">
+      <c r="Q19" t="s">
         <v>963</v>
       </c>
-      <c r="R19" s="43" t="s">
+      <c r="R19" t="s">
         <v>963</v>
       </c>
       <c r="S19" s="7">
@@ -45937,13 +45875,13 @@
       <c r="O20" t="s">
         <v>5029</v>
       </c>
-      <c r="P20" s="43" t="s">
+      <c r="P20" t="s">
         <v>963</v>
       </c>
-      <c r="Q20" s="42" t="s">
+      <c r="Q20" t="s">
         <v>963</v>
       </c>
-      <c r="R20" s="43" t="s">
+      <c r="R20" t="s">
         <v>963</v>
       </c>
       <c r="S20" s="7">
@@ -45996,13 +45934,13 @@
       <c r="O21" t="s">
         <v>5029</v>
       </c>
-      <c r="P21" s="43" t="s">
+      <c r="P21" t="s">
         <v>963</v>
       </c>
-      <c r="Q21" s="42" t="s">
+      <c r="Q21" t="s">
         <v>963</v>
       </c>
-      <c r="R21" s="43" t="s">
+      <c r="R21" t="s">
         <v>963</v>
       </c>
       <c r="S21" s="7">
@@ -46055,13 +45993,13 @@
       <c r="O22" t="s">
         <v>5029</v>
       </c>
-      <c r="P22" s="43" t="s">
+      <c r="P22" t="s">
         <v>963</v>
       </c>
-      <c r="Q22" s="42" t="s">
+      <c r="Q22" t="s">
         <v>963</v>
       </c>
-      <c r="R22" s="43" t="s">
+      <c r="R22" t="s">
         <v>963</v>
       </c>
       <c r="S22" s="7">
@@ -46114,13 +46052,13 @@
       <c r="O23" t="s">
         <v>5029</v>
       </c>
-      <c r="P23" s="43" t="s">
+      <c r="P23" t="s">
         <v>966</v>
       </c>
-      <c r="Q23" s="42" t="s">
+      <c r="Q23" t="s">
         <v>963</v>
       </c>
-      <c r="R23" s="43" t="s">
+      <c r="R23" t="s">
         <v>966</v>
       </c>
       <c r="S23" s="7" t="s">
@@ -46176,13 +46114,13 @@
       <c r="O24" t="s">
         <v>5029</v>
       </c>
-      <c r="P24" s="43" t="s">
+      <c r="P24" t="s">
         <v>963</v>
       </c>
-      <c r="Q24" s="42" t="s">
+      <c r="Q24" t="s">
         <v>963</v>
       </c>
-      <c r="R24" s="43" t="s">
+      <c r="R24" t="s">
         <v>963</v>
       </c>
       <c r="S24" s="7">
@@ -46235,13 +46173,13 @@
       <c r="O25" t="s">
         <v>5029</v>
       </c>
-      <c r="P25" s="43" t="s">
+      <c r="P25" t="s">
         <v>963</v>
       </c>
-      <c r="Q25" s="42" t="s">
+      <c r="Q25" t="s">
         <v>963</v>
       </c>
-      <c r="R25" s="43" t="s">
+      <c r="R25" t="s">
         <v>963</v>
       </c>
       <c r="S25" s="7">
@@ -46294,13 +46232,13 @@
       <c r="O26" t="s">
         <v>5029</v>
       </c>
-      <c r="P26" s="43" t="s">
+      <c r="P26" t="s">
         <v>963</v>
       </c>
-      <c r="Q26" s="42" t="s">
+      <c r="Q26" t="s">
         <v>963</v>
       </c>
-      <c r="R26" s="43" t="s">
+      <c r="R26" t="s">
         <v>963</v>
       </c>
       <c r="S26" s="7">
@@ -46353,13 +46291,13 @@
       <c r="O27" t="s">
         <v>5029</v>
       </c>
-      <c r="P27" s="43" t="s">
+      <c r="P27" t="s">
         <v>963</v>
       </c>
-      <c r="Q27" s="42" t="s">
+      <c r="Q27" t="s">
         <v>963</v>
       </c>
-      <c r="R27" s="43" t="s">
+      <c r="R27" t="s">
         <v>963</v>
       </c>
       <c r="S27" s="7">
@@ -46415,10 +46353,10 @@
       <c r="P28" t="s">
         <v>963</v>
       </c>
-      <c r="Q28" s="42" t="s">
+      <c r="Q28" t="s">
         <v>963</v>
       </c>
-      <c r="R28" s="43" t="s">
+      <c r="R28" t="s">
         <v>963</v>
       </c>
       <c r="S28" s="7">
@@ -46474,10 +46412,10 @@
       <c r="P29" t="s">
         <v>966</v>
       </c>
-      <c r="Q29" s="42" t="s">
+      <c r="Q29" t="s">
         <v>963</v>
       </c>
-      <c r="R29" s="43" t="s">
+      <c r="R29" t="s">
         <v>966</v>
       </c>
       <c r="S29" s="7" t="s">
@@ -46533,10 +46471,10 @@
       <c r="P30" t="s">
         <v>963</v>
       </c>
-      <c r="Q30" s="42" t="s">
+      <c r="Q30" t="s">
         <v>963</v>
       </c>
-      <c r="R30" s="43" t="s">
+      <c r="R30" t="s">
         <v>963</v>
       </c>
       <c r="S30" s="7">
@@ -46595,10 +46533,10 @@
       <c r="P31" t="s">
         <v>963</v>
       </c>
-      <c r="Q31" s="42" t="s">
+      <c r="Q31" t="s">
         <v>963</v>
       </c>
-      <c r="R31" s="43" t="s">
+      <c r="R31" t="s">
         <v>963</v>
       </c>
       <c r="S31" s="7">
@@ -46654,10 +46592,10 @@
       <c r="P32" t="s">
         <v>963</v>
       </c>
-      <c r="Q32" s="42" t="s">
+      <c r="Q32" t="s">
         <v>963</v>
       </c>
-      <c r="R32" s="43" t="s">
+      <c r="R32" t="s">
         <v>963</v>
       </c>
       <c r="S32" s="7">
@@ -46713,10 +46651,10 @@
       <c r="P33" t="s">
         <v>963</v>
       </c>
-      <c r="Q33" s="42" t="s">
+      <c r="Q33" t="s">
         <v>963</v>
       </c>
-      <c r="R33" s="43" t="s">
+      <c r="R33" t="s">
         <v>963</v>
       </c>
       <c r="S33" s="7">
@@ -46772,10 +46710,10 @@
       <c r="P34" t="s">
         <v>5373</v>
       </c>
-      <c r="Q34" s="42" t="s">
+      <c r="Q34" t="s">
         <v>963</v>
       </c>
-      <c r="R34" s="43" t="s">
+      <c r="R34" t="s">
         <v>966</v>
       </c>
       <c r="S34" s="7" t="s">
@@ -46831,388 +46769,412 @@
       <c r="P35" t="s">
         <v>963</v>
       </c>
-      <c r="Q35" s="42" t="s">
+      <c r="Q35" t="s">
         <v>963</v>
       </c>
-      <c r="R35" s="43" t="s">
+      <c r="R35" t="s">
         <v>963</v>
       </c>
       <c r="S35" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="40">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" t="s">
         <v>5282</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C36" t="s">
         <v>5283</v>
       </c>
-      <c r="D36" s="40">
+      <c r="D36">
         <v>1993</v>
       </c>
-      <c r="E36" s="40" t="s">
+      <c r="E36" t="s">
         <v>5284</v>
       </c>
-      <c r="F36" s="40" t="s">
+      <c r="F36" t="s">
         <v>5285</v>
       </c>
-      <c r="G36" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H36" s="40" t="s">
+      <c r="G36" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H36" t="s">
         <v>99</v>
       </c>
-      <c r="I36" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J36" s="40" t="s">
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
         <v>5349</v>
       </c>
-      <c r="K36" s="40" t="s">
+      <c r="K36" t="s">
         <v>5349</v>
       </c>
-      <c r="L36" s="40">
+      <c r="L36">
         <v>1442</v>
       </c>
-      <c r="M36" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N36" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O36" s="40" t="s">
+      <c r="M36" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N36" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O36" t="s">
         <v>5029</v>
       </c>
       <c r="P36" t="s">
         <v>963</v>
       </c>
-      <c r="Q36" s="42" t="s">
+      <c r="Q36" t="s">
         <v>963</v>
       </c>
-      <c r="R36" s="43" t="s">
+      <c r="R36" t="s">
         <v>963</v>
       </c>
-      <c r="S36" s="41">
+      <c r="S36" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="40">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" t="s">
         <v>469</v>
       </c>
-      <c r="C37" s="40" t="s">
+      <c r="C37" t="s">
         <v>470</v>
       </c>
-      <c r="D37" s="40">
+      <c r="D37">
         <v>2006</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" t="s">
         <v>5286</v>
       </c>
-      <c r="F37" s="40" t="s">
+      <c r="F37" t="s">
         <v>5287</v>
       </c>
-      <c r="G37" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H37" s="40" t="s">
+      <c r="G37" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H37" t="s">
         <v>477</v>
       </c>
-      <c r="I37" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J37" s="40" t="s">
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
         <v>5349</v>
       </c>
-      <c r="K37" s="40" t="s">
+      <c r="K37" t="s">
         <v>5349</v>
       </c>
-      <c r="L37" s="40">
+      <c r="L37">
         <v>254</v>
       </c>
-      <c r="M37" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N37" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O37" s="40" t="s">
+      <c r="M37" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N37" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O37" t="s">
         <v>5029</v>
       </c>
       <c r="P37" t="s">
         <v>963</v>
       </c>
-      <c r="Q37" s="42" t="s">
+      <c r="Q37" t="s">
         <v>963</v>
       </c>
-      <c r="R37" s="43" t="s">
+      <c r="R37" t="s">
         <v>963</v>
       </c>
-      <c r="S37" s="41">
+      <c r="S37" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="40">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" t="s">
         <v>472</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" t="s">
         <v>473</v>
       </c>
-      <c r="D38" s="40">
+      <c r="D38">
         <v>1998</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" t="s">
         <v>5288</v>
       </c>
-      <c r="F38" s="40" t="s">
+      <c r="F38" t="s">
         <v>5289</v>
       </c>
-      <c r="G38" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H38" s="40" t="s">
+      <c r="G38" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H38" t="s">
         <v>19</v>
       </c>
-      <c r="I38" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" s="40" t="s">
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
         <v>5349</v>
       </c>
-      <c r="K38" s="40" t="s">
+      <c r="K38" t="s">
         <v>5349</v>
       </c>
-      <c r="L38" s="40">
+      <c r="L38">
         <v>301</v>
       </c>
-      <c r="M38" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N38" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O38" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q38" s="42" t="s">
+      <c r="M38" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N38" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O38" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P38" t="s">
         <v>963</v>
       </c>
-      <c r="S38" s="41"/>
-    </row>
-    <row r="39" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="40">
+      <c r="Q38" t="s">
+        <v>963</v>
+      </c>
+      <c r="R38" t="s">
+        <v>963</v>
+      </c>
+      <c r="S38" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" t="s">
         <v>475</v>
       </c>
-      <c r="C39" s="40" t="s">
+      <c r="C39" t="s">
         <v>476</v>
       </c>
-      <c r="D39" s="40">
+      <c r="D39">
         <v>2001</v>
       </c>
-      <c r="E39" s="40" t="s">
+      <c r="E39" t="s">
         <v>5290</v>
       </c>
-      <c r="F39" s="40" t="s">
+      <c r="F39" t="s">
         <v>5291</v>
       </c>
-      <c r="G39" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H39" s="40" t="s">
+      <c r="G39" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H39" t="s">
         <v>5361</v>
       </c>
-      <c r="I39" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J39" s="40" t="s">
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" t="s">
         <v>5349</v>
       </c>
-      <c r="K39" s="40" t="s">
+      <c r="K39" t="s">
         <v>5349</v>
       </c>
-      <c r="L39" s="40">
+      <c r="L39">
         <v>293</v>
       </c>
-      <c r="M39" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N39" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O39" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q39" s="42" t="s">
+      <c r="M39" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N39" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O39" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P39" t="s">
+        <v>5375</v>
+      </c>
+      <c r="Q39" t="s">
         <v>963</v>
       </c>
-      <c r="S39" s="41"/>
-    </row>
-    <row r="40" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="40">
+      <c r="R39" t="s">
+        <v>966</v>
+      </c>
+      <c r="S39" s="7" t="s">
+        <v>5029</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" t="s">
         <v>3923</v>
       </c>
-      <c r="C40" s="40" t="s">
+      <c r="C40" t="s">
         <v>3924</v>
       </c>
-      <c r="D40" s="40">
+      <c r="D40">
         <v>2008</v>
       </c>
-      <c r="E40" s="40" t="s">
+      <c r="E40" t="s">
         <v>5292</v>
       </c>
-      <c r="F40" s="40" t="s">
+      <c r="F40" t="s">
         <v>5293</v>
       </c>
-      <c r="G40" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H40" s="40" t="s">
+      <c r="G40" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H40" t="s">
         <v>5359</v>
       </c>
-      <c r="I40" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J40" s="40" t="s">
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" t="s">
         <v>5349</v>
       </c>
-      <c r="K40" s="40" t="s">
+      <c r="K40" t="s">
         <v>5349</v>
       </c>
-      <c r="L40" s="40">
+      <c r="L40">
         <v>153</v>
       </c>
-      <c r="M40" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N40" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O40" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q40" s="42" t="s">
+      <c r="M40" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N40" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O40" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P40" t="s">
         <v>963</v>
       </c>
-      <c r="S40" s="41"/>
-    </row>
-    <row r="41" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="40">
+      <c r="Q40" t="s">
+        <v>963</v>
+      </c>
+      <c r="R40" t="s">
+        <v>963</v>
+      </c>
+      <c r="S40" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="40" t="s">
+      <c r="B41" t="s">
         <v>5294</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="C41" t="s">
         <v>5295</v>
       </c>
-      <c r="D41" s="40">
+      <c r="D41">
         <v>2001</v>
       </c>
-      <c r="E41" s="40" t="s">
+      <c r="E41" t="s">
         <v>5296</v>
       </c>
-      <c r="F41" s="40" t="s">
+      <c r="F41" t="s">
         <v>5297</v>
       </c>
-      <c r="G41" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H41" s="40" t="s">
+      <c r="G41" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H41" t="s">
         <v>42</v>
       </c>
-      <c r="I41" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J41" s="40" t="s">
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" t="s">
         <v>5349</v>
       </c>
-      <c r="K41" s="40" t="s">
+      <c r="K41" t="s">
         <v>5349</v>
       </c>
-      <c r="L41" s="40">
+      <c r="L41">
         <v>188</v>
       </c>
-      <c r="M41" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N41" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O41" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q41" s="42" t="s">
+      <c r="M41" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N41" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O41" t="s">
+        <v>5029</v>
+      </c>
+      <c r="Q41" t="s">
         <v>963</v>
       </c>
-      <c r="S41" s="41"/>
-    </row>
-    <row r="42" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="40">
+      <c r="S41" s="7"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" t="s">
         <v>5298</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" t="s">
         <v>5299</v>
       </c>
-      <c r="D42" s="40">
+      <c r="D42">
         <v>2004</v>
       </c>
-      <c r="E42" s="40" t="s">
+      <c r="E42" t="s">
         <v>5300</v>
       </c>
-      <c r="F42" s="40" t="s">
+      <c r="F42" t="s">
         <v>5301</v>
       </c>
-      <c r="G42" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H42" s="40" t="s">
+      <c r="G42" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H42" t="s">
         <v>5354</v>
       </c>
-      <c r="I42" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J42" s="40" t="s">
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" t="s">
         <v>5349</v>
       </c>
-      <c r="K42" s="40" t="s">
+      <c r="K42" t="s">
         <v>5349</v>
       </c>
-      <c r="L42" s="40">
+      <c r="L42">
         <v>93</v>
       </c>
-      <c r="M42" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N42" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O42" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q42" s="42" t="s">
+      <c r="M42" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N42" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O42" t="s">
+        <v>5029</v>
+      </c>
+      <c r="Q42" t="s">
         <v>963</v>
       </c>
-      <c r="S42" s="41"/>
+      <c r="S42" s="7"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -47260,7 +47222,7 @@
       <c r="O43" t="s">
         <v>5029</v>
       </c>
-      <c r="Q43" s="42" t="s">
+      <c r="Q43" t="s">
         <v>963</v>
       </c>
       <c r="S43" s="7"/>
@@ -47311,7 +47273,7 @@
       <c r="O44" t="s">
         <v>5029</v>
       </c>
-      <c r="Q44" s="42" t="s">
+      <c r="Q44" t="s">
         <v>963</v>
       </c>
       <c r="S44" s="7"/>
@@ -47362,7 +47324,7 @@
       <c r="O45" t="s">
         <v>5029</v>
       </c>
-      <c r="Q45" s="42" t="s">
+      <c r="Q45" t="s">
         <v>963</v>
       </c>
       <c r="S45" s="7"/>
@@ -47413,7 +47375,7 @@
       <c r="O46" t="s">
         <v>5029</v>
       </c>
-      <c r="Q46" s="42" t="s">
+      <c r="Q46" t="s">
         <v>963</v>
       </c>
       <c r="S46" s="7"/>
@@ -47464,7 +47426,7 @@
       <c r="O47" t="s">
         <v>5029</v>
       </c>
-      <c r="Q47" s="42" t="s">
+      <c r="Q47" t="s">
         <v>963</v>
       </c>
       <c r="S47" s="7"/>
@@ -47515,7 +47477,7 @@
       <c r="O48" t="s">
         <v>5029</v>
       </c>
-      <c r="Q48" s="42" t="s">
+      <c r="Q48" t="s">
         <v>963</v>
       </c>
       <c r="S48" s="7"/>
@@ -47566,7 +47528,7 @@
       <c r="O49" t="s">
         <v>5029</v>
       </c>
-      <c r="Q49" s="42" t="s">
+      <c r="Q49" t="s">
         <v>963</v>
       </c>
       <c r="S49" s="7"/>
@@ -47617,7 +47579,7 @@
       <c r="O50" t="s">
         <v>5029</v>
       </c>
-      <c r="Q50" s="42" t="s">
+      <c r="Q50" t="s">
         <v>963</v>
       </c>
       <c r="S50" s="7"/>
@@ -47668,7 +47630,7 @@
       <c r="O51" t="s">
         <v>5029</v>
       </c>
-      <c r="Q51" s="42" t="s">
+      <c r="Q51" t="s">
         <v>963</v>
       </c>
       <c r="S51" s="7"/>
@@ -47719,7 +47681,7 @@
       <c r="O52" t="s">
         <v>5029</v>
       </c>
-      <c r="Q52" s="42" t="s">
+      <c r="Q52" t="s">
         <v>963</v>
       </c>
       <c r="S52" s="7"/>
@@ -47770,7 +47732,7 @@
       <c r="O53" t="s">
         <v>5029</v>
       </c>
-      <c r="Q53" s="42" t="s">
+      <c r="Q53" t="s">
         <v>963</v>
       </c>
       <c r="S53" s="7"/>
@@ -47821,7 +47783,7 @@
       <c r="O54" t="s">
         <v>5029</v>
       </c>
-      <c r="Q54" s="42" t="s">
+      <c r="Q54" t="s">
         <v>963</v>
       </c>
       <c r="S54" s="7"/>
@@ -47872,7 +47834,7 @@
       <c r="O55" t="s">
         <v>5029</v>
       </c>
-      <c r="Q55" s="42" t="s">
+      <c r="Q55" t="s">
         <v>963</v>
       </c>
       <c r="S55" s="7"/>
@@ -47923,7 +47885,7 @@
       <c r="O56" t="s">
         <v>5029</v>
       </c>
-      <c r="Q56" s="42" t="s">
+      <c r="Q56" t="s">
         <v>963</v>
       </c>
       <c r="S56" s="7"/>
@@ -49488,43 +49450,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="45" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="44" priority="13">
+    <cfRule type="containsBlanks" dxfId="35" priority="13">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:R601">
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="34" priority="8" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",P2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="12" priority="9" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="33" priority="9" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",P2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="32" priority="10" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",P2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S601">
-    <cfRule type="containsBlanks" dxfId="43" priority="15">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="between">
+      <formula>1</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="7" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",S2)))</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="29" priority="15">
       <formula>LEN(TRIM(S2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S601">
-    <cfRule type="cellIs" dxfId="42" priority="6" operator="between">
-      <formula>1</formula>
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="7" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",S2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="U1:U2">
-    <cfRule type="duplicateValues" dxfId="40" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1">
-    <cfRule type="duplicateValues" dxfId="39" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -49533,12 +49493,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Z19"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50555,127 +50515,91 @@
         <v>5374</v>
       </c>
     </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M23" s="41"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="38" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="37" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="duplicateValues" dxfId="24" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="containsBlanks" dxfId="36" priority="33">
+    <cfRule type="containsBlanks" dxfId="23" priority="33">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
-    <cfRule type="containsBlanks" dxfId="35" priority="22">
+  <conditionalFormatting sqref="F18:F19">
+    <cfRule type="containsBlanks" dxfId="22" priority="11">
       <formula>LEN(TRIM(F18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H17 H20:H1048576">
-    <cfRule type="containsBlanks" dxfId="34" priority="34">
+    <cfRule type="containsBlanks" dxfId="21" priority="34">
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="duplicateValues" dxfId="33" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="duplicateValues" dxfId="32" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O18">
-    <cfRule type="containsText" dxfId="31" priority="19" operator="containsText" text="PRIMARY STUDY">
+  <conditionalFormatting sqref="L19">
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:O19">
+    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="30" priority="20" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="16" priority="9" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="21" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18">
-    <cfRule type="cellIs" dxfId="28" priority="17" operator="between">
+  <conditionalFormatting sqref="O18:O19">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="18" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",O18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18:P18">
-    <cfRule type="containsBlanks" dxfId="26" priority="15">
+  <conditionalFormatting sqref="O18:P19">
+    <cfRule type="containsBlanks" dxfId="12" priority="4">
       <formula>LEN(TRIM(O18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P18 P20:P1048576">
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="between">
+  <conditionalFormatting sqref="P1:P1048576">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="14" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1 Q4">
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="28" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="8" priority="29" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",Q1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R2">
-    <cfRule type="duplicateValues" dxfId="21" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="duplicateValues" dxfId="20" priority="25"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F19">
-    <cfRule type="containsBlanks" dxfId="9" priority="11">
-      <formula>LEN(TRIM(F19))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L19">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M19:O19">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="PRIMARY STUDY">
-      <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M19)))</formula>
-    </cfRule>
-    <cfRule type="notContainsText" dxfId="6" priority="9" operator="notContains" text="YES">
-      <formula>ISERROR(SEARCH("YES",M19))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="YES">
-      <formula>NOT(ISERROR(SEARCH("YES",M19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O19">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
-      <formula>1</formula>
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",O19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O19:P19">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
-      <formula>LEN(TRIM(O19))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P19">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
-      <formula>1</formula>
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",P19)))</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" dxfId="6" priority="25"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -50684,7 +50608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L251"/>
   <sheetViews>
@@ -59568,10 +59492,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1 A1:K251">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$K1=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>$J1=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -59582,7 +59506,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M293"/>
   <sheetViews>
@@ -67516,10 +67440,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:J253 J257 J259:J1048576">
-    <cfRule type="containsText" dxfId="17" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67536,10 +67460,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",M17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",M17)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67548,7 +67472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Finished gathering the raw snoballing data. Wage info, automatic data still to add.
</commit_message>
<xml_diff>
--- a/Data/Snowballing/snowballing_Literature.xlsx
+++ b/Data/Snowballing/snowballing_Literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Data\Snowballing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E133AF0F-E218-44C4-8672-6FA0EFC4637C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5E70D0-705B-463D-A2C5-D0FBFE4454E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10224" uniqueCount="5376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10275" uniqueCount="5374">
   <si>
     <t>Number</t>
   </si>
@@ -16600,12 +16600,6 @@
   </si>
   <si>
     <t>Light, A. and Strayer, W. (2004): "Who Receives the College Wage Premium Assessing the Labor Market Returns to Degrees and College Transfer Patterns." The Journal of Human Resources, 39(3), pp. 746-773.</t>
-  </si>
-  <si>
-    <t>Miller, &amp; Nmartin(1995): (1995)</t>
-  </si>
-  <si>
-    <t>Miller, &amp; Nmartin(1995):</t>
   </si>
   <si>
     <t>What do Twins Studies Reveal About the Economic Returns to Education?</t>
@@ -17119,15 +17113,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -17152,6 +17137,17 @@
       <bottom style="dotted">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -17200,20 +17196,48 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="71">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8CDC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -17253,6 +17277,126 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC5C5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8CDC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6161"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8CDC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6161"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17993,7 +18137,7 @@
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!S1</f>
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5039</v>
@@ -18224,7 +18368,7 @@
       <c r="T5" s="2" t="s">
         <v>5140</v>
       </c>
-      <c r="U5" s="38">
+      <c r="U5" s="37">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
         <v>74</v>
       </c>
@@ -18330,7 +18474,7 @@
         <v>5029</v>
       </c>
       <c r="P7" t="s">
-        <v>5371</v>
+        <v>5369</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>904</v>
@@ -18485,37 +18629,37 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
+      <c r="A11" s="38">
         <v>10</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>3935</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="38" t="s">
         <v>3936</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="38">
         <v>2005</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="38" t="s">
         <v>1072</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="38" t="s">
         <v>970</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="38" t="s">
         <v>1074</v>
       </c>
-      <c r="H11" s="39">
-        <v>1</v>
-      </c>
-      <c r="I11" s="39" t="s">
+      <c r="H11" s="38">
+        <v>1</v>
+      </c>
+      <c r="I11" s="38" t="s">
         <v>1073</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="38" t="s">
         <v>1075</v>
       </c>
-      <c r="K11" s="39" t="s">
+      <c r="K11" s="38" t="s">
         <v>1075</v>
       </c>
       <c r="L11" t="s">
@@ -19847,37 +19991,37 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="39">
+      <c r="A38" s="38">
         <v>37</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="38" t="s">
         <v>3965</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="38" t="s">
         <v>3966</v>
       </c>
-      <c r="D38" s="39">
+      <c r="D38" s="38">
         <v>2003</v>
       </c>
-      <c r="E38" s="39" t="s">
+      <c r="E38" s="38" t="s">
         <v>1211</v>
       </c>
-      <c r="F38" s="39" t="s">
+      <c r="F38" s="38" t="s">
         <v>4598</v>
       </c>
-      <c r="G38" s="39" t="s">
+      <c r="G38" s="38" t="s">
         <v>1213</v>
       </c>
-      <c r="H38" s="39">
+      <c r="H38" s="38">
         <v>265</v>
       </c>
-      <c r="I38" s="39" t="s">
+      <c r="I38" s="38" t="s">
         <v>1212</v>
       </c>
-      <c r="J38" s="39" t="s">
+      <c r="J38" s="38" t="s">
         <v>1214</v>
       </c>
-      <c r="K38" s="39" t="s">
+      <c r="K38" s="38" t="s">
         <v>1215</v>
       </c>
       <c r="L38" t="s">
@@ -28041,53 +28185,53 @@
         <v>904</v>
       </c>
     </row>
-    <row r="201" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="36">
+    <row r="201" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="35">
         <v>200</v>
       </c>
-      <c r="B201" s="36" t="s">
+      <c r="B201" s="35" t="s">
         <v>4141</v>
       </c>
-      <c r="C201" s="36" t="s">
+      <c r="C201" s="35" t="s">
         <v>4142</v>
       </c>
-      <c r="D201" s="36">
+      <c r="D201" s="35">
         <v>4903</v>
       </c>
-      <c r="E201" s="36" t="s">
+      <c r="E201" s="35" t="s">
         <v>2025</v>
       </c>
-      <c r="F201" s="36" t="s">
+      <c r="F201" s="35" t="s">
         <v>4621</v>
       </c>
-      <c r="G201" s="36" t="s">
+      <c r="G201" s="35" t="s">
         <v>2027</v>
       </c>
-      <c r="H201" s="36">
+      <c r="H201" s="35">
         <v>7</v>
       </c>
-      <c r="I201" s="36" t="s">
+      <c r="I201" s="35" t="s">
         <v>2026</v>
       </c>
-      <c r="J201" s="36" t="s">
+      <c r="J201" s="35" t="s">
         <v>2028</v>
       </c>
-      <c r="K201" s="36" t="s">
+      <c r="K201" s="35" t="s">
         <v>2028</v>
       </c>
-      <c r="L201" s="36" t="s">
+      <c r="L201" s="35" t="s">
         <v>974</v>
       </c>
-      <c r="M201" s="36" t="s">
+      <c r="M201" s="35" t="s">
         <v>966</v>
       </c>
-      <c r="N201" s="36" t="s">
+      <c r="N201" s="35" t="s">
         <v>966</v>
       </c>
-      <c r="O201" s="37" t="s">
-        <v>5029</v>
-      </c>
-      <c r="R201" s="36" t="s">
+      <c r="O201" s="36" t="s">
+        <v>5029</v>
+      </c>
+      <c r="R201" s="35" t="s">
         <v>904</v>
       </c>
     </row>
@@ -44567,59 +44711,59 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="50" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="49" priority="20">
+    <cfRule type="containsBlanks" dxfId="69" priority="20">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N601">
-    <cfRule type="containsText" dxfId="48" priority="11" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="68" priority="11" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",L2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="47" priority="12" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="67" priority="12" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",L2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="13" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="66" priority="13" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O601 P136 P146 P151 P161 P163 P177 P187 P189:P190">
-    <cfRule type="containsBlanks" dxfId="45" priority="22">
+    <cfRule type="containsBlanks" dxfId="65" priority="22">
       <formula>LEN(TRIM(O2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O601 P177 P187 P189:P190">
-    <cfRule type="cellIs" dxfId="44" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="64" priority="8" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="63" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q10 Q16:Q1048576 R11:R15">
-    <cfRule type="duplicateValues" dxfId="42" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="41" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="40" priority="23">
+    <cfRule type="containsBlanks" dxfId="60" priority="23">
       <formula>LEN(TRIM(R6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8">
-    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="58" priority="18" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="duplicateValues" dxfId="37" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="5"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K160" r:id="rId1" location="page=11" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -44637,8 +44781,8 @@
   <dimension ref="A1:AC575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44715,7 +44859,7 @@
       <c r="S1" s="25" t="s">
         <v>5137</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="T1" s="39" t="s">
         <v>5145</v>
       </c>
       <c r="U1" s="28" t="s">
@@ -44730,7 +44874,7 @@
       </c>
       <c r="Y1" s="29">
         <f>COUNTIF($P:$P, "YES")</f>
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="Z1" s="31"/>
       <c r="AA1" s="31"/>
@@ -44766,10 +44910,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L2" s="34">
         <v>289</v>
@@ -44826,16 +44970,16 @@
         <v>5029</v>
       </c>
       <c r="H3" t="s">
-        <v>5350</v>
+        <v>5348</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K3" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L3">
         <v>1486</v>
@@ -44850,7 +44994,7 @@
         <v>5029</v>
       </c>
       <c r="P3" t="s">
-        <v>5366</v>
+        <v>5364</v>
       </c>
       <c r="Q3" t="s">
         <v>963</v>
@@ -44891,10 +45035,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K4" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L4">
         <v>321</v>
@@ -44944,16 +45088,16 @@
         <v>5029</v>
       </c>
       <c r="H5" t="s">
-        <v>5351</v>
+        <v>5349</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K5" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L5">
         <v>3590</v>
@@ -45009,10 +45153,10 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K6" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L6">
         <v>1510</v>
@@ -45039,14 +45183,14 @@
         <v>5029</v>
       </c>
       <c r="T6" t="s">
-        <v>5364</v>
+        <v>5362</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>5143</v>
       </c>
       <c r="V6">
         <f>COUNTIF($P:$P, "YES")</f>
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
@@ -45072,16 +45216,16 @@
         <v>5029</v>
       </c>
       <c r="H7" t="s">
-        <v>5352</v>
+        <v>5350</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K7" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L7">
         <v>321</v>
@@ -45112,7 +45256,7 @@
       </c>
       <c r="V7">
         <f>COUNTIFS($R:$R, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
@@ -45144,10 +45288,10 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K8" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L8">
         <v>588</v>
@@ -45197,16 +45341,16 @@
         <v>5029</v>
       </c>
       <c r="H9" t="s">
-        <v>5353</v>
+        <v>5351</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K9" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L9">
         <v>73</v>
@@ -45256,16 +45400,16 @@
         <v>5029</v>
       </c>
       <c r="H10" t="s">
-        <v>5354</v>
+        <v>5352</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K10" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L10">
         <v>74</v>
@@ -45280,7 +45424,7 @@
         <v>5029</v>
       </c>
       <c r="P10" t="s">
-        <v>5365</v>
+        <v>5363</v>
       </c>
       <c r="Q10" t="s">
         <v>963</v>
@@ -45321,10 +45465,10 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K11" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L11">
         <v>17</v>
@@ -45374,16 +45518,16 @@
         <v>5029</v>
       </c>
       <c r="H12" t="s">
-        <v>5355</v>
+        <v>5353</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K12" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L12">
         <v>1789</v>
@@ -45433,16 +45577,16 @@
         <v>5029</v>
       </c>
       <c r="H13" t="s">
-        <v>5352</v>
+        <v>5350</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K13" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L13">
         <v>2928</v>
@@ -45457,7 +45601,7 @@
         <v>5029</v>
       </c>
       <c r="P13" t="s">
-        <v>5367</v>
+        <v>5365</v>
       </c>
       <c r="Q13" t="s">
         <v>963</v>
@@ -45469,7 +45613,7 @@
         <v>1</v>
       </c>
       <c r="T13" t="s">
-        <v>5368</v>
+        <v>5366</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -45495,16 +45639,16 @@
         <v>5029</v>
       </c>
       <c r="H14" t="s">
-        <v>5356</v>
+        <v>5354</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K14" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L14">
         <v>783</v>
@@ -45554,16 +45698,16 @@
         <v>5029</v>
       </c>
       <c r="H15" t="s">
-        <v>5357</v>
+        <v>5355</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K15" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L15">
         <v>141</v>
@@ -45590,7 +45734,7 @@
         <v>5029</v>
       </c>
       <c r="T15" t="s">
-        <v>5369</v>
+        <v>5367</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
@@ -45622,10 +45766,10 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K16" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L16">
         <v>284</v>
@@ -45675,16 +45819,16 @@
         <v>5029</v>
       </c>
       <c r="H17" t="s">
-        <v>5358</v>
+        <v>5356</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K17" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L17">
         <v>252</v>
@@ -45740,10 +45884,10 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K18" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L18">
         <v>88</v>
@@ -45799,10 +45943,10 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K19" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L19">
         <v>2852</v>
@@ -45858,10 +46002,10 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K20" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L20">
         <v>386</v>
@@ -45911,16 +46055,16 @@
         <v>5029</v>
       </c>
       <c r="H21" t="s">
-        <v>5359</v>
+        <v>5357</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K21" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L21">
         <v>494</v>
@@ -45976,10 +46120,10 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K22" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L22">
         <v>101</v>
@@ -46029,16 +46173,16 @@
         <v>5029</v>
       </c>
       <c r="H23" t="s">
-        <v>5354</v>
+        <v>5352</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K23" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L23">
         <v>92</v>
@@ -46065,7 +46209,7 @@
         <v>5029</v>
       </c>
       <c r="T23" t="s">
-        <v>5370</v>
+        <v>5368</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -46097,10 +46241,10 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K24" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L24">
         <v>171</v>
@@ -46150,16 +46294,16 @@
         <v>5029</v>
       </c>
       <c r="H25" t="s">
-        <v>5359</v>
+        <v>5357</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K25" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L25">
         <v>662</v>
@@ -46215,10 +46359,10 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K26" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L26">
         <v>888</v>
@@ -46274,10 +46418,10 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K27" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L27">
         <v>100</v>
@@ -46327,16 +46471,16 @@
         <v>5029</v>
       </c>
       <c r="H28" t="s">
-        <v>5354</v>
+        <v>5352</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K28" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L28">
         <v>860</v>
@@ -46392,10 +46536,10 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K29" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L29">
         <v>27</v>
@@ -46445,16 +46589,16 @@
         <v>5029</v>
       </c>
       <c r="H30" t="s">
-        <v>5360</v>
+        <v>5358</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K30" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L30">
         <v>1427</v>
@@ -46481,7 +46625,7 @@
         <v>3</v>
       </c>
       <c r="T30" t="s">
-        <v>5372</v>
+        <v>5370</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -46507,16 +46651,16 @@
         <v>5029</v>
       </c>
       <c r="H31" t="s">
-        <v>5359</v>
+        <v>5357</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K31" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L31">
         <v>80</v>
@@ -46572,10 +46716,10 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K32" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L32">
         <v>182</v>
@@ -46625,16 +46769,16 @@
         <v>5029</v>
       </c>
       <c r="H33" t="s">
-        <v>5354</v>
+        <v>5352</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K33" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L33">
         <v>389</v>
@@ -46690,10 +46834,10 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K34" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L34">
         <v>177</v>
@@ -46708,7 +46852,7 @@
         <v>5029</v>
       </c>
       <c r="P34" t="s">
-        <v>5373</v>
+        <v>5371</v>
       </c>
       <c r="Q34" t="s">
         <v>963</v>
@@ -46749,10 +46893,10 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K35" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L35">
         <v>217</v>
@@ -46808,10 +46952,10 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K36" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L36">
         <v>1442</v>
@@ -46867,10 +47011,10 @@
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K37" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L37">
         <v>254</v>
@@ -46926,10 +47070,10 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K38" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L38">
         <v>301</v>
@@ -46979,16 +47123,16 @@
         <v>5029</v>
       </c>
       <c r="H39" t="s">
-        <v>5361</v>
+        <v>5359</v>
       </c>
       <c r="I39" t="b">
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K39" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L39">
         <v>293</v>
@@ -47003,7 +47147,7 @@
         <v>5029</v>
       </c>
       <c r="P39" t="s">
-        <v>5375</v>
+        <v>5373</v>
       </c>
       <c r="Q39" t="s">
         <v>963</v>
@@ -47038,16 +47182,16 @@
         <v>5029</v>
       </c>
       <c r="H40" t="s">
-        <v>5359</v>
+        <v>5357</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K40" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L40">
         <v>153</v>
@@ -47103,10 +47247,10 @@
         <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K41" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L41">
         <v>188</v>
@@ -47120,10 +47264,18 @@
       <c r="O41" t="s">
         <v>5029</v>
       </c>
+      <c r="P41" t="s">
+        <v>963</v>
+      </c>
       <c r="Q41" t="s">
         <v>963</v>
       </c>
-      <c r="S41" s="7"/>
+      <c r="R41" t="s">
+        <v>963</v>
+      </c>
+      <c r="S41" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -47148,16 +47300,16 @@
         <v>5029</v>
       </c>
       <c r="H42" t="s">
-        <v>5354</v>
+        <v>5352</v>
       </c>
       <c r="I42" t="b">
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K42" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L42">
         <v>93</v>
@@ -47171,44 +47323,52 @@
       <c r="O42" t="s">
         <v>5029</v>
       </c>
+      <c r="P42" t="s">
+        <v>963</v>
+      </c>
       <c r="Q42" t="s">
         <v>963</v>
       </c>
-      <c r="S42" s="7"/>
+      <c r="R42" t="s">
+        <v>963</v>
+      </c>
+      <c r="S42" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>5302</v>
+        <v>5073</v>
       </c>
       <c r="C43" t="s">
-        <v>5303</v>
+        <v>4128</v>
       </c>
       <c r="D43">
         <v>1995</v>
       </c>
       <c r="E43" t="s">
-        <v>5304</v>
+        <v>5302</v>
       </c>
       <c r="F43" t="s">
-        <v>5305</v>
+        <v>5303</v>
       </c>
       <c r="G43" t="s">
         <v>5029</v>
       </c>
       <c r="H43" t="s">
-        <v>5362</v>
+        <v>5360</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K43" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L43">
         <v>372</v>
@@ -47222,29 +47382,37 @@
       <c r="O43" t="s">
         <v>5029</v>
       </c>
+      <c r="P43" t="s">
+        <v>5371</v>
+      </c>
       <c r="Q43" t="s">
         <v>963</v>
       </c>
-      <c r="S43" s="7"/>
+      <c r="R43" t="s">
+        <v>966</v>
+      </c>
+      <c r="S43" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>5306</v>
+        <v>5304</v>
       </c>
       <c r="C44" t="s">
-        <v>5307</v>
+        <v>5305</v>
       </c>
       <c r="D44">
         <v>2004</v>
       </c>
       <c r="E44" t="s">
-        <v>5308</v>
+        <v>5306</v>
       </c>
       <c r="F44" t="s">
-        <v>5309</v>
+        <v>5307</v>
       </c>
       <c r="G44" t="s">
         <v>5029</v>
@@ -47256,10 +47424,10 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K44" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L44">
         <v>1830</v>
@@ -47273,29 +47441,37 @@
       <c r="O44" t="s">
         <v>5029</v>
       </c>
+      <c r="P44" t="s">
+        <v>963</v>
+      </c>
       <c r="Q44" t="s">
         <v>963</v>
       </c>
-      <c r="S44" s="7"/>
+      <c r="R44" t="s">
+        <v>963</v>
+      </c>
+      <c r="S44" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>5310</v>
+        <v>5308</v>
       </c>
       <c r="C45" t="s">
-        <v>5311</v>
+        <v>5309</v>
       </c>
       <c r="D45">
         <v>2005</v>
       </c>
       <c r="E45" t="s">
-        <v>5312</v>
+        <v>5310</v>
       </c>
       <c r="F45" t="s">
-        <v>5313</v>
+        <v>5311</v>
       </c>
       <c r="G45" t="s">
         <v>5029</v>
@@ -47307,10 +47483,10 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K45" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L45">
         <v>345</v>
@@ -47324,44 +47500,52 @@
       <c r="O45" t="s">
         <v>5029</v>
       </c>
+      <c r="P45" t="s">
+        <v>963</v>
+      </c>
       <c r="Q45" t="s">
         <v>963</v>
       </c>
-      <c r="S45" s="7"/>
+      <c r="R45" t="s">
+        <v>963</v>
+      </c>
+      <c r="S45" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>5314</v>
+        <v>5312</v>
       </c>
       <c r="C46" t="s">
-        <v>5315</v>
+        <v>5313</v>
       </c>
       <c r="D46">
         <v>2006</v>
       </c>
       <c r="E46" t="s">
-        <v>5316</v>
+        <v>5314</v>
       </c>
       <c r="F46" t="s">
-        <v>5317</v>
+        <v>5315</v>
       </c>
       <c r="G46" t="s">
         <v>5029</v>
       </c>
       <c r="H46" t="s">
-        <v>5363</v>
+        <v>5361</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K46" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L46">
         <v>1005</v>
@@ -47375,29 +47559,37 @@
       <c r="O46" t="s">
         <v>5029</v>
       </c>
+      <c r="P46" t="s">
+        <v>5363</v>
+      </c>
       <c r="Q46" t="s">
         <v>963</v>
       </c>
-      <c r="S46" s="7"/>
+      <c r="R46" t="s">
+        <v>966</v>
+      </c>
+      <c r="S46" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>5318</v>
+        <v>5316</v>
       </c>
       <c r="C47" t="s">
-        <v>5319</v>
+        <v>5317</v>
       </c>
       <c r="D47">
         <v>2006</v>
       </c>
       <c r="E47" t="s">
-        <v>5320</v>
+        <v>5318</v>
       </c>
       <c r="F47" t="s">
-        <v>5321</v>
+        <v>5319</v>
       </c>
       <c r="G47" t="s">
         <v>5029</v>
@@ -47409,10 +47601,10 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K47" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L47">
         <v>596</v>
@@ -47426,26 +47618,34 @@
       <c r="O47" t="s">
         <v>5029</v>
       </c>
+      <c r="P47" t="s">
+        <v>5363</v>
+      </c>
       <c r="Q47" t="s">
         <v>963</v>
       </c>
-      <c r="S47" s="7"/>
+      <c r="R47" t="s">
+        <v>966</v>
+      </c>
+      <c r="S47" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>5322</v>
+        <v>5320</v>
       </c>
       <c r="C48" t="s">
-        <v>5323</v>
+        <v>5321</v>
       </c>
       <c r="D48">
         <v>2005</v>
       </c>
       <c r="E48" t="s">
-        <v>5324</v>
+        <v>5322</v>
       </c>
       <c r="F48" t="s">
         <v>5164</v>
@@ -47460,10 +47660,10 @@
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K48" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L48">
         <v>386</v>
@@ -47477,10 +47677,18 @@
       <c r="O48" t="s">
         <v>5029</v>
       </c>
+      <c r="P48" t="s">
+        <v>963</v>
+      </c>
       <c r="Q48" t="s">
         <v>963</v>
       </c>
-      <c r="S48" s="7"/>
+      <c r="R48" t="s">
+        <v>963</v>
+      </c>
+      <c r="S48" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49">
@@ -47496,7 +47704,7 @@
         <v>1982</v>
       </c>
       <c r="E49" t="s">
-        <v>5325</v>
+        <v>5323</v>
       </c>
       <c r="F49" t="s">
         <v>5165</v>
@@ -47505,16 +47713,16 @@
         <v>5029</v>
       </c>
       <c r="H49" t="s">
-        <v>5362</v>
+        <v>5360</v>
       </c>
       <c r="I49" t="b">
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K49" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L49">
         <v>55</v>
@@ -47528,10 +47736,18 @@
       <c r="O49" t="s">
         <v>5029</v>
       </c>
+      <c r="P49" t="s">
+        <v>963</v>
+      </c>
       <c r="Q49" t="s">
         <v>963</v>
       </c>
-      <c r="S49" s="7"/>
+      <c r="R49" t="s">
+        <v>963</v>
+      </c>
+      <c r="S49" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50">
@@ -47547,7 +47763,7 @@
         <v>1985</v>
       </c>
       <c r="E50" t="s">
-        <v>5326</v>
+        <v>5324</v>
       </c>
       <c r="F50" t="s">
         <v>5166</v>
@@ -47562,10 +47778,10 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K50" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L50">
         <v>2143</v>
@@ -47579,17 +47795,25 @@
       <c r="O50" t="s">
         <v>5029</v>
       </c>
+      <c r="P50" t="s">
+        <v>974</v>
+      </c>
       <c r="Q50" t="s">
         <v>963</v>
       </c>
-      <c r="S50" s="7"/>
+      <c r="R50" t="s">
+        <v>966</v>
+      </c>
+      <c r="S50" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>5327</v>
+        <v>5325</v>
       </c>
       <c r="C51" t="s">
         <v>674</v>
@@ -47598,7 +47822,7 @@
         <v>1979</v>
       </c>
       <c r="E51" t="s">
-        <v>5328</v>
+        <v>5326</v>
       </c>
       <c r="F51" t="s">
         <v>5167</v>
@@ -47613,10 +47837,10 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K51" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L51">
         <v>251</v>
@@ -47630,29 +47854,37 @@
       <c r="O51" t="s">
         <v>5029</v>
       </c>
+      <c r="P51" t="s">
+        <v>963</v>
+      </c>
       <c r="Q51" t="s">
         <v>963</v>
       </c>
-      <c r="S51" s="7"/>
+      <c r="R51" t="s">
+        <v>963</v>
+      </c>
+      <c r="S51" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>5329</v>
+        <v>5327</v>
       </c>
       <c r="C52" t="s">
-        <v>5330</v>
+        <v>5328</v>
       </c>
       <c r="D52">
         <v>1997</v>
       </c>
       <c r="E52" t="s">
-        <v>5331</v>
+        <v>5329</v>
       </c>
       <c r="F52" t="s">
-        <v>5332</v>
+        <v>5330</v>
       </c>
       <c r="G52" t="s">
         <v>5029</v>
@@ -47664,10 +47896,10 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K52" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L52">
         <v>9699</v>
@@ -47681,44 +47913,52 @@
       <c r="O52" t="s">
         <v>5029</v>
       </c>
+      <c r="P52" t="s">
+        <v>963</v>
+      </c>
       <c r="Q52" t="s">
         <v>963</v>
       </c>
-      <c r="S52" s="7"/>
+      <c r="R52" t="s">
+        <v>963</v>
+      </c>
+      <c r="S52" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>5333</v>
+        <v>5331</v>
       </c>
       <c r="C53" t="s">
-        <v>5334</v>
+        <v>5332</v>
       </c>
       <c r="D53">
         <v>2014</v>
       </c>
       <c r="E53" t="s">
-        <v>5335</v>
+        <v>5333</v>
       </c>
       <c r="F53" t="s">
-        <v>5336</v>
+        <v>5334</v>
       </c>
       <c r="G53" t="s">
         <v>5029</v>
       </c>
       <c r="H53" t="s">
-        <v>5352</v>
+        <v>5350</v>
       </c>
       <c r="I53" t="b">
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K53" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L53">
         <v>264</v>
@@ -47732,29 +47972,37 @@
       <c r="O53" t="s">
         <v>5029</v>
       </c>
+      <c r="P53" t="s">
+        <v>963</v>
+      </c>
       <c r="Q53" t="s">
         <v>963</v>
       </c>
-      <c r="S53" s="7"/>
+      <c r="R53" t="s">
+        <v>963</v>
+      </c>
+      <c r="S53" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>5337</v>
+        <v>5335</v>
       </c>
       <c r="C54" t="s">
-        <v>5338</v>
+        <v>5336</v>
       </c>
       <c r="D54">
         <v>2001</v>
       </c>
       <c r="E54" t="s">
-        <v>5339</v>
+        <v>5337</v>
       </c>
       <c r="F54" t="s">
-        <v>5340</v>
+        <v>5338</v>
       </c>
       <c r="G54" t="s">
         <v>5029</v>
@@ -47766,10 +48014,10 @@
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K54" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L54">
         <v>261</v>
@@ -47783,29 +48031,37 @@
       <c r="O54" t="s">
         <v>5029</v>
       </c>
+      <c r="P54" t="s">
+        <v>963</v>
+      </c>
       <c r="Q54" t="s">
         <v>963</v>
       </c>
-      <c r="S54" s="7"/>
+      <c r="R54" t="s">
+        <v>963</v>
+      </c>
+      <c r="S54" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>5341</v>
+        <v>5339</v>
       </c>
       <c r="C55" t="s">
-        <v>5342</v>
+        <v>5340</v>
       </c>
       <c r="D55">
         <v>1999</v>
       </c>
       <c r="E55" t="s">
-        <v>5343</v>
+        <v>5341</v>
       </c>
       <c r="F55" t="s">
-        <v>5344</v>
+        <v>5342</v>
       </c>
       <c r="G55" t="s">
         <v>5029</v>
@@ -47817,10 +48073,10 @@
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K55" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L55">
         <v>423</v>
@@ -47834,29 +48090,37 @@
       <c r="O55" t="s">
         <v>5029</v>
       </c>
+      <c r="P55" t="s">
+        <v>963</v>
+      </c>
       <c r="Q55" t="s">
         <v>963</v>
       </c>
-      <c r="S55" s="7"/>
+      <c r="R55" t="s">
+        <v>963</v>
+      </c>
+      <c r="S55" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>5345</v>
+        <v>5343</v>
       </c>
       <c r="C56" t="s">
-        <v>5346</v>
+        <v>5344</v>
       </c>
       <c r="D56">
         <v>2011</v>
       </c>
       <c r="E56" t="s">
-        <v>5347</v>
+        <v>5345</v>
       </c>
       <c r="F56" t="s">
-        <v>5348</v>
+        <v>5346</v>
       </c>
       <c r="G56" t="s">
         <v>5029</v>
@@ -47868,10 +48132,10 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K56" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L56">
         <v>197</v>
@@ -47885,10 +48149,18 @@
       <c r="O56" t="s">
         <v>5029</v>
       </c>
+      <c r="P56" t="s">
+        <v>966</v>
+      </c>
       <c r="Q56" t="s">
         <v>963</v>
       </c>
-      <c r="S56" s="7"/>
+      <c r="R56" t="s">
+        <v>966</v>
+      </c>
+      <c r="S56" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S57" s="7"/>
@@ -48323,8 +48595,8 @@
     <row r="200" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S200" s="7"/>
     </row>
-    <row r="201" spans="19:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="S201" s="37"/>
+    <row r="201" spans="19:19" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S201" s="36"/>
     </row>
     <row r="202" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S202" s="7"/>
@@ -49450,41 +49722,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="36" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="35" priority="13">
+    <cfRule type="containsBlanks" dxfId="55" priority="13">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:R601">
-    <cfRule type="containsText" dxfId="34" priority="8" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="54" priority="8" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",P2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="33" priority="9" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="53" priority="9" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",P2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="10" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="52" priority="10" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",P2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S601">
-    <cfRule type="cellIs" dxfId="31" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="51" priority="6" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="7" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="50" priority="7" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",S2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="29" priority="15">
+    <cfRule type="containsBlanks" dxfId="49" priority="15">
       <formula>LEN(TRIM(S2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U2">
-    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1">
-    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -49498,7 +49770,7 @@
   <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49563,7 +49835,7 @@
       </c>
       <c r="S1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5039</v>
@@ -49623,7 +49895,7 @@
       <c r="O2" t="s">
         <v>966</v>
       </c>
-      <c r="P2" s="35">
+      <c r="P2" s="41">
         <v>1</v>
       </c>
       <c r="S2" t="s">
@@ -49679,7 +49951,7 @@
       <c r="O3" t="s">
         <v>966</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="7">
         <v>1</v>
       </c>
       <c r="X3" t="s">
@@ -49732,7 +50004,7 @@
       <c r="O4" t="s">
         <v>966</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="7">
         <v>1</v>
       </c>
       <c r="Q4" t="s">
@@ -49788,7 +50060,7 @@
       <c r="O5" t="s">
         <v>966</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="7">
         <v>1</v>
       </c>
     </row>
@@ -49838,7 +50110,7 @@
       <c r="O6" t="s">
         <v>966</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="7">
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
@@ -49846,7 +50118,7 @@
       </c>
       <c r="S6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="X6" t="s">
         <v>5076</v>
@@ -49898,7 +50170,7 @@
       <c r="O7" t="s">
         <v>966</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="7">
         <v>1</v>
       </c>
       <c r="R7" s="2" t="s">
@@ -49955,7 +50227,7 @@
       <c r="O8" t="s">
         <v>966</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="7">
         <v>1</v>
       </c>
     </row>
@@ -50002,7 +50274,7 @@
       <c r="O9" t="s">
         <v>966</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="7">
         <v>1</v>
       </c>
     </row>
@@ -50052,7 +50324,7 @@
       <c r="O10" t="s">
         <v>966</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="7">
         <v>1</v>
       </c>
     </row>
@@ -50099,7 +50371,7 @@
       <c r="O11" t="s">
         <v>966</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="7">
         <v>1</v>
       </c>
     </row>
@@ -50149,7 +50421,7 @@
       <c r="O12" t="s">
         <v>966</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="7">
         <v>1</v>
       </c>
     </row>
@@ -50199,7 +50471,7 @@
       <c r="O13" t="s">
         <v>966</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="7" t="s">
         <v>5121</v>
       </c>
     </row>
@@ -50249,7 +50521,7 @@
       <c r="O14" t="s">
         <v>966</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="7">
         <v>1</v>
       </c>
     </row>
@@ -50299,7 +50571,7 @@
       <c r="O15" t="s">
         <v>966</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="7">
         <v>1</v>
       </c>
     </row>
@@ -50349,7 +50621,7 @@
       <c r="O16" t="s">
         <v>966</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="7">
         <v>1</v>
       </c>
       <c r="Q16" t="s">
@@ -50402,7 +50674,7 @@
       <c r="O17" t="s">
         <v>966</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="7">
         <v>1</v>
       </c>
       <c r="Q17" t="s">
@@ -50455,7 +50727,7 @@
       <c r="O18" t="s">
         <v>966</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="7">
         <v>1</v>
       </c>
       <c r="Q18" t="s">
@@ -50508,98 +50780,167 @@
       <c r="O19" t="s">
         <v>966</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="7" t="s">
         <v>5029</v>
       </c>
       <c r="Q19" t="s">
-        <v>5374</v>
+        <v>5372</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5073</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4128</v>
+      </c>
+      <c r="D20">
+        <v>1995</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5302</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5303</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H20">
+        <v>372</v>
+      </c>
+      <c r="I20" t="s">
+        <v>5029</v>
+      </c>
+      <c r="J20" t="s">
+        <v>5029</v>
+      </c>
+      <c r="K20" t="s">
+        <v>5029</v>
+      </c>
+      <c r="L20" t="s">
+        <v>5073</v>
+      </c>
+      <c r="M20" t="s">
+        <v>5371</v>
+      </c>
+      <c r="N20" t="s">
+        <v>963</v>
+      </c>
+      <c r="O20" t="s">
+        <v>966</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>5029</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>5372</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M23" s="41"/>
+      <c r="M23" s="40"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="26" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="25" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="24" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="containsBlanks" dxfId="23" priority="33">
+    <cfRule type="containsBlanks" dxfId="43" priority="37">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:F19">
-    <cfRule type="containsBlanks" dxfId="22" priority="11">
+    <cfRule type="containsBlanks" dxfId="42" priority="15">
       <formula>LEN(TRIM(F18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H17 H20:H1048576">
-    <cfRule type="containsBlanks" dxfId="21" priority="34">
+    <cfRule type="containsBlanks" dxfId="41" priority="38">
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="duplicateValues" dxfId="20" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="duplicateValues" dxfId="19" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O19">
-    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="37" priority="12" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="16" priority="9" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="36" priority="13" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="35" priority="14" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18:O19">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
+  <conditionalFormatting sqref="O18:O20">
+    <cfRule type="cellIs" dxfId="34" priority="10" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="33" priority="11" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",O18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O18:P19">
-    <cfRule type="containsBlanks" dxfId="12" priority="4">
+    <cfRule type="containsBlanks" dxfId="32" priority="8">
       <formula>LEN(TRIM(O18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="30" priority="7" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1 Q4">
-    <cfRule type="cellIs" dxfId="9" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="32" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="29" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",Q1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R2">
-    <cfRule type="duplicateValues" dxfId="7" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="duplicateValues" dxfId="6" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M20:O20">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="PRIMARY STUDY">
+      <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M20)))</formula>
+    </cfRule>
+    <cfRule type="notContainsText" dxfId="2" priority="3" operator="notContains" text="YES">
+      <formula>ISERROR(SEARCH("YES",M20))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",M20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20:P20">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(O20))=0</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -59492,10 +59833,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1 A1:K251">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>$K1=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$J1=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67440,10 +67781,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:J253 J257 J259:J1048576">
-    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="6" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67460,10 +67801,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",M17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",M17)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added source min_wage/med_exp data
</commit_message>
<xml_diff>
--- a/Data/Snowballing/snowballing_Literature.xlsx
+++ b/Data/Snowballing/snowballing_Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Data\Snowballing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5E70D0-705B-463D-A2C5-D0FBFE4454E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077E15AB-E6A0-4E37-AA6D-05DCA5F0EA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44782,7 +44782,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>